<commit_message>
Perbaikan Klast dan PCA
</commit_message>
<xml_diff>
--- a/R/assets/Data Total No R.xlsx
+++ b/R/assets/Data Total No R.xlsx
@@ -684,7 +684,7 @@
         <v>26.13</v>
       </c>
       <c r="U2" s="5">
-        <v>307.4233</v>
+        <v>299.96</v>
       </c>
       <c r="V2" s="5">
         <v>6.426667</v>
@@ -761,7 +761,7 @@
         <v>27.21</v>
       </c>
       <c r="U3" s="5">
-        <v>294.6133</v>
+        <v>285.55</v>
       </c>
       <c r="V3" s="5">
         <v>8.686667</v>
@@ -838,7 +838,7 @@
         <v>25.08</v>
       </c>
       <c r="U4" s="5">
-        <v>299.9567</v>
+        <v>354.79</v>
       </c>
       <c r="V4" s="5">
         <v>7.173333</v>
@@ -915,7 +915,7 @@
         <v>27.58</v>
       </c>
       <c r="U5" s="5">
-        <v>285.5467</v>
+        <v>441.2</v>
       </c>
       <c r="V5" s="5">
         <v>6.47</v>
@@ -992,7 +992,7 @@
         <v>31.32</v>
       </c>
       <c r="U6" s="5">
-        <v>354.7867</v>
+        <v>453.19</v>
       </c>
       <c r="V6" s="5">
         <v>7.68</v>
@@ -1069,7 +1069,7 @@
         <v>20.5</v>
       </c>
       <c r="U7" s="5">
-        <v>441.1967</v>
+        <v>360.17</v>
       </c>
       <c r="V7" s="5">
         <v>8.273333</v>
@@ -1146,7 +1146,7 @@
         <v>38.19</v>
       </c>
       <c r="U8" s="5">
-        <v>380.96</v>
+        <v>269.65</v>
       </c>
       <c r="V8" s="5">
         <v>6.766667</v>
@@ -1223,7 +1223,7 @@
         <v>32.32</v>
       </c>
       <c r="U9" s="5">
-        <v>360.1733</v>
+        <v>293.42</v>
       </c>
       <c r="V9" s="5">
         <v>7.85</v>
@@ -1300,7 +1300,7 @@
         <v>15.17</v>
       </c>
       <c r="U10" s="5">
-        <v>269.6533</v>
+        <v>263.66</v>
       </c>
       <c r="V10" s="5">
         <v>6.506667</v>
@@ -1377,7 +1377,7 @@
         <v>30.06</v>
       </c>
       <c r="U11" s="5">
-        <v>293.42</v>
+        <v>333.76</v>
       </c>
       <c r="V11" s="5">
         <v>7.343333</v>
@@ -1454,7 +1454,7 @@
         <v>35.21</v>
       </c>
       <c r="U12" s="5">
-        <v>263.6567</v>
+        <v>307.42</v>
       </c>
       <c r="V12" s="5">
         <v>7.256667</v>
@@ -1531,7 +1531,7 @@
         <v>29.73</v>
       </c>
       <c r="U13" s="5">
-        <v>333.7567</v>
+        <v>294.61</v>
       </c>
       <c r="V13" s="5">
         <v>6.976667</v>

</xml_diff>

<commit_message>
R: Add new post hoc test & genotipe names
</commit_message>
<xml_diff>
--- a/R/assets/Data Total No R.xlsx
+++ b/R/assets/Data Total No R.xlsx
@@ -91,40 +91,40 @@
     <t>B100</t>
   </si>
   <si>
-    <t>G32</t>
-  </si>
-  <si>
-    <t>G33</t>
-  </si>
-  <si>
-    <t>G11</t>
-  </si>
-  <si>
-    <t>G12</t>
-  </si>
-  <si>
-    <t>G13</t>
-  </si>
-  <si>
-    <t>G14</t>
-  </si>
-  <si>
-    <t>G15</t>
-  </si>
-  <si>
-    <t>G16</t>
-  </si>
-  <si>
-    <t>G17</t>
-  </si>
-  <si>
-    <t>G18</t>
-  </si>
-  <si>
-    <t>G19</t>
-  </si>
-  <si>
-    <t>G20</t>
+    <t>Argopuro</t>
+  </si>
+  <si>
+    <t>Grobogan</t>
+  </si>
+  <si>
+    <t>UBASK31</t>
+  </si>
+  <si>
+    <t>UBASK36</t>
+  </si>
+  <si>
+    <t>UBASK34</t>
+  </si>
+  <si>
+    <t>UBASK32</t>
+  </si>
+  <si>
+    <t>UBASK35</t>
+  </si>
+  <si>
+    <t>UBASK41</t>
+  </si>
+  <si>
+    <t>UBASK46</t>
+  </si>
+  <si>
+    <t>UBASK43</t>
+  </si>
+  <si>
+    <t>UBASK42</t>
+  </si>
+  <si>
+    <t>UBASK45</t>
   </si>
 </sst>
 </file>

</xml_diff>